<commit_message>
"quoth the raven never more"
</commit_message>
<xml_diff>
--- a/ExtractedFeatures/Features_with_respect_to_trials.xlsx
+++ b/ExtractedFeatures/Features_with_respect_to_trials.xlsx
@@ -1146,196 +1146,214 @@
         <v>202</v>
       </c>
       <c r="C3">
-        <v>-0.0432398275306608</v>
+        <v>-0.06778564228962507</v>
       </c>
       <c r="D3">
-        <v>-0.5707121914329751</v>
+        <v>-0.6473335752170566</v>
       </c>
       <c r="E3">
-        <v>0.5405302440458183</v>
+        <v>0.5493948348744779</v>
       </c>
       <c r="F3">
-        <v>0.07554041409641568</v>
+        <v>0.06853313509662716</v>
       </c>
       <c r="G3">
-        <v>-0.4439584742365437</v>
+        <v>-0.4539519709241162</v>
       </c>
       <c r="H3">
-        <v>0.4152942276076048</v>
+        <v>0.4222925583339146</v>
       </c>
       <c r="I3">
-        <v>-0.03310191570800388</v>
+        <v>-0.01318125193054271</v>
       </c>
       <c r="J3">
-        <v>-0.2780685372024321</v>
+        <v>0.9636801478230531</v>
       </c>
       <c r="K3">
-        <v>0.04417552783349819</v>
+        <v>0.02831260680176752</v>
+      </c>
+      <c r="L3">
+        <v>0.06040454062648083</v>
+      </c>
+      <c r="M3">
+        <v>-0.4947404136212541</v>
+      </c>
+      <c r="N3">
+        <v>0.4341926614871541</v>
+      </c>
+      <c r="O3">
+        <v>-0.06040454658422392</v>
+      </c>
+      <c r="P3">
+        <v>-0.4947401954287738</v>
+      </c>
+      <c r="Q3">
+        <v>0.5658073389676668</v>
       </c>
       <c r="R3">
-        <v>22.18949390818336</v>
+        <v>19.20749420500179</v>
       </c>
       <c r="S3">
-        <v>-0.7496128697410149</v>
+        <v>-0.8909745524311108</v>
       </c>
       <c r="T3">
-        <v>270.0845782929611</v>
+        <v>270.7502469379378</v>
       </c>
       <c r="U3">
-        <v>-0.3181329422530481</v>
+        <v>-0.2706257499234986</v>
       </c>
       <c r="V3">
-        <v>279.2175178792895</v>
+        <v>278.3452178247458</v>
       </c>
       <c r="Z3">
-        <v>1.256046102036741</v>
+        <v>1.288391225169693</v>
       </c>
       <c r="AA3">
-        <v>40.46253244005602</v>
+        <v>40.80399446376837</v>
       </c>
       <c r="AE3">
-        <v>1.158048213961562</v>
+        <v>1.187869740427624</v>
       </c>
       <c r="AF3">
-        <v>22.90224152057319</v>
+        <v>23.09551280799815</v>
       </c>
       <c r="AJ3">
-        <v>0.6795065371477246</v>
+        <v>0.6970048778360557</v>
       </c>
       <c r="AO3">
-        <v>0.004176552980711554</v>
+        <v>0.004284105657490979</v>
       </c>
       <c r="AP3">
-        <v>0.1398067217091019</v>
+        <v>0.1409865461848463</v>
       </c>
       <c r="AT3">
-        <v>0.003850694422749282</v>
+        <v>0.003949855739399389</v>
       </c>
       <c r="AU3">
-        <v>0.07913215297448106</v>
+        <v>0.079799946695386</v>
       </c>
       <c r="AY3">
-        <v>0.002259467266794878</v>
+        <v>0.002317652031542643</v>
       </c>
       <c r="BA3">
-        <v>1.022673977489637</v>
+        <v>0.9848193982062357</v>
       </c>
       <c r="BB3">
-        <v>0.6133333689658065</v>
+        <v>0.7328930431439958</v>
       </c>
       <c r="BC3">
-        <v>12.3568558745364</v>
+        <v>12.44645988964466</v>
       </c>
       <c r="BD3">
-        <v>-0.03289802722978617</v>
+        <v>-0.02670952659263602</v>
       </c>
       <c r="BE3">
-        <v>13.33715846994536</v>
+        <v>13.23220338983051</v>
       </c>
       <c r="BF3">
-        <v>1.709781879459464</v>
+        <v>1.619311068683604</v>
       </c>
       <c r="BG3">
-        <v>-0.2371198100551327</v>
+        <v>-0.2760595240799184</v>
       </c>
       <c r="BH3">
-        <v>5.373360587638374</v>
+        <v>5.465107967864329</v>
       </c>
       <c r="BI3">
-        <v>-0.06751875520978054</v>
+        <v>-0.06189362945645832</v>
       </c>
       <c r="BJ3">
-        <v>7.358469945355193</v>
+        <v>7.252542372881357</v>
       </c>
       <c r="BK3">
-        <v>-1.169495715952253</v>
+        <v>-1.457444750963728</v>
       </c>
       <c r="BL3">
-        <v>-1.060582109806696</v>
+        <v>-1.044297698570743</v>
       </c>
       <c r="BM3">
-        <v>6.449657524010748</v>
+        <v>6.554914141061038</v>
       </c>
       <c r="BN3">
-        <v>0.0308419005279244</v>
+        <v>0.04091174751607241</v>
       </c>
       <c r="BO3">
-        <v>5.556830601092898</v>
+        <v>5.389830508474576</v>
       </c>
       <c r="BP3">
-        <v>-0.256317809691282</v>
+        <v>-0.1852502881121705</v>
       </c>
       <c r="BQ3">
-        <v>0.1183577488567059</v>
+        <v>1.040731765825411</v>
       </c>
       <c r="BR3">
-        <v>0.5338377780395962</v>
+        <v>0.4264377837557281</v>
       </c>
       <c r="BS3">
-        <v>0.003778827452070011</v>
+        <v>-0.005727644652250154</v>
       </c>
       <c r="BT3">
-        <v>0.4218579234972681</v>
+        <v>0.5898305084745763</v>
       </c>
       <c r="BU3">
-        <v>0.07712781662773986</v>
+        <v>0.07013598475023911</v>
       </c>
       <c r="BV3">
-        <v>-0.4143920018701035</v>
+        <v>-0.439494650126642</v>
       </c>
       <c r="BW3">
-        <v>0.4163045324516773</v>
+        <v>0.4233399886896293</v>
       </c>
       <c r="BX3">
-        <v>-0.003350358157628542</v>
+        <v>-0.002816439246258236</v>
       </c>
       <c r="BY3">
-        <v>0.5146225274412608</v>
+        <v>0.5045109365732364</v>
       </c>
       <c r="BZ3">
-        <v>-0.04722785884087668</v>
+        <v>-0.07172491627521779</v>
       </c>
       <c r="CA3">
-        <v>-0.5737571349908618</v>
+        <v>-0.6628430903675414</v>
       </c>
       <c r="CB3">
-        <v>0.5336397738240869</v>
+        <v>0.5423709256652932</v>
       </c>
       <c r="CC3">
-        <v>0.002387224349805112</v>
+        <v>0.003235143316032676</v>
       </c>
       <c r="CD3">
-        <v>0.4636439034103099</v>
+        <v>0.4492998489837577</v>
       </c>
       <c r="CE3">
-        <v>-0.03140579342120419</v>
+        <v>-0.01588796965796603</v>
       </c>
       <c r="CF3">
-        <v>-0.1734276191277216</v>
+        <v>1.119177552663611</v>
       </c>
       <c r="CG3">
-        <v>0.05005569237268088</v>
+        <v>0.03428908589053887</v>
       </c>
       <c r="CH3">
-        <v>0.000963133807823423</v>
+        <v>-0.0004187040697744526</v>
       </c>
       <c r="CI3">
-        <v>0.02173356914842986</v>
+        <v>0.04618921444300571</v>
       </c>
       <c r="CJ3">
-        <v>0.2637386169057753</v>
+        <v>0.1764054364261761</v>
       </c>
       <c r="CK3">
-        <v>-0.6394763463575919</v>
+        <v>-0.5700887690516562</v>
       </c>
       <c r="CL3">
-        <v>3.019289878579862</v>
+        <v>3.052461139162825</v>
       </c>
       <c r="CM3">
-        <v>-0.01130869686023898</v>
+        <v>-0.008766803039158428</v>
       </c>
       <c r="CN3">
-        <v>3.350273224043718</v>
+        <v>3.305084745762713</v>
       </c>
     </row>
     <row r="4" spans="1:92">
@@ -2702,196 +2720,232 @@
         <v>209</v>
       </c>
       <c r="C10">
-        <v>0.04246490407066619</v>
+        <v>0.04594943933365733</v>
       </c>
       <c r="D10">
-        <v>0.7989015431737019</v>
+        <v>1.074912531447437</v>
       </c>
       <c r="E10">
-        <v>0.4489747402085732</v>
+        <v>0.4564152473620577</v>
       </c>
       <c r="F10">
-        <v>0.03917845758227507</v>
+        <v>0.0244044040211456</v>
       </c>
       <c r="G10">
-        <v>-0.112261015810127</v>
+        <v>-0.008021278785228942</v>
       </c>
       <c r="H10">
-        <v>0.4407128967023826</v>
+        <v>0.448111535110376</v>
       </c>
       <c r="I10">
-        <v>-0.07333043925891594</v>
+        <v>-0.06130373665863323</v>
       </c>
       <c r="J10">
-        <v>0.3630403445069675</v>
+        <v>0.7155785127028472</v>
       </c>
       <c r="K10">
-        <v>0.1103123626682717</v>
+        <v>0.09547320969296454</v>
+      </c>
+      <c r="L10">
+        <v>0.0256641040484506</v>
+      </c>
+      <c r="M10">
+        <v>-0.9680906120826636</v>
+      </c>
+      <c r="N10">
+        <v>0.4874862825823784</v>
+      </c>
+      <c r="O10">
+        <v>-0.02566410606166351</v>
+      </c>
+      <c r="P10">
+        <v>-0.9680904241389079</v>
+      </c>
+      <c r="Q10">
+        <v>0.5125137174503233</v>
       </c>
       <c r="R10">
-        <v>20.44240517965986</v>
+        <v>19.68630553591419</v>
       </c>
       <c r="S10">
-        <v>1.278130978459525</v>
+        <v>1.242702135667751</v>
       </c>
       <c r="T10">
-        <v>278.8086552165456</v>
+        <v>279.4974579697418</v>
       </c>
       <c r="U10">
-        <v>1.188648160767028</v>
+        <v>1.271501404109685</v>
       </c>
       <c r="V10">
-        <v>244.0697538001202</v>
+        <v>242.9397850870029</v>
+      </c>
+      <c r="W10">
+        <v>26.50902810630701</v>
+      </c>
+      <c r="X10">
+        <v>1.203454915746716</v>
+      </c>
+      <c r="Y10">
+        <v>276.8657744925675</v>
       </c>
       <c r="Z10">
-        <v>0.8404671248142086</v>
+        <v>1.327268597059798</v>
       </c>
       <c r="AA10">
-        <v>27.17672414033745</v>
+        <v>238.7943155145231</v>
       </c>
       <c r="AE10">
-        <v>1.257228618272821</v>
+        <v>1.289604193021523</v>
       </c>
       <c r="AF10">
-        <v>34.35497602392071</v>
+        <v>34.64489657338449</v>
       </c>
       <c r="AK10">
-        <v>36.41895339883708</v>
+        <v>36.72629178769042</v>
+      </c>
+      <c r="AL10">
+        <v>-0.01381004801219559</v>
+      </c>
+      <c r="AM10">
+        <v>-1.545264415494619</v>
+      </c>
+      <c r="AN10">
+        <v>0.9851059480952336</v>
       </c>
       <c r="AO10">
-        <v>0.002881087090953902</v>
+        <v>0.00032775304165062</v>
       </c>
       <c r="AP10">
-        <v>0.1143370958717503</v>
+        <v>0.9758351022102892</v>
       </c>
       <c r="AT10">
-        <v>0.004309728525412991</v>
+        <v>0.004420710677738483</v>
       </c>
       <c r="AU10">
-        <v>0.1445372211542024</v>
+        <v>0.1457569661642358</v>
       </c>
       <c r="AZ10">
-        <v>0.1532207246469088</v>
+        <v>0.1545137494666013</v>
       </c>
       <c r="BA10">
-        <v>0.5716231032314688</v>
+        <v>0.5731573103274017</v>
       </c>
       <c r="BB10">
-        <v>-0.1857280642947883</v>
+        <v>-0.2976183881606958</v>
       </c>
       <c r="BC10">
-        <v>15.48509261895313</v>
+        <v>15.47742500097059</v>
       </c>
       <c r="BD10">
-        <v>-0.01708808002222851</v>
+        <v>-0.01788427819988324</v>
       </c>
       <c r="BE10">
-        <v>15.98743169398908</v>
+        <v>15.99322033898305</v>
       </c>
       <c r="BF10">
-        <v>0.9941130884745026</v>
+        <v>0.7610745062273941</v>
       </c>
       <c r="BG10">
-        <v>-0.6518782487798008</v>
+        <v>-0.7973505130943954</v>
       </c>
       <c r="BH10">
-        <v>6.776718485443276</v>
+        <v>6.89058567184697</v>
       </c>
       <c r="BI10">
-        <v>-0.01872742428452354</v>
+        <v>-0.009234365867913617</v>
       </c>
       <c r="BJ10">
-        <v>7.319125683060114</v>
+        <v>7.149152542372884</v>
       </c>
       <c r="BK10">
-        <v>0.8749699964977941</v>
+        <v>0.8942249191081975</v>
       </c>
       <c r="BL10">
-        <v>0.7695410516463397</v>
+        <v>0.971624588937006</v>
       </c>
       <c r="BM10">
-        <v>7.073186518153011</v>
+        <v>7.190873666392797</v>
       </c>
       <c r="BN10">
-        <v>-0.01119755487635461</v>
+        <v>-0.0006428988895383258</v>
       </c>
       <c r="BO10">
-        <v>7.413661202185795</v>
+        <v>7.222033898305084</v>
       </c>
       <c r="BP10">
-        <v>-0.864095729423674</v>
+        <v>-0.6076219650536202</v>
       </c>
       <c r="BQ10">
-        <v>0.129114370222855</v>
+        <v>0.6381644647234</v>
       </c>
       <c r="BR10">
-        <v>1.635187624644807</v>
+        <v>1.395965660347877</v>
       </c>
       <c r="BS10">
-        <v>0.01283689913864963</v>
+        <v>-0.008007013442431338</v>
       </c>
       <c r="BT10">
-        <v>1.25464480874317</v>
+        <v>1.622033898305085</v>
       </c>
       <c r="BU10">
-        <v>0.03829519209564029</v>
+        <v>0.02305447746770857</v>
       </c>
       <c r="BV10">
-        <v>-0.4616658049090657</v>
+        <v>-0.533297627246399</v>
       </c>
       <c r="BW10">
-        <v>0.4335149109647731</v>
+        <v>0.4407721488581078</v>
       </c>
       <c r="BX10">
-        <v>-0.0004956125749418873</v>
+        <v>0.0001151750045676211</v>
       </c>
       <c r="BY10">
-        <v>0.4478511783593498</v>
+        <v>0.4372334239169262</v>
       </c>
       <c r="BZ10">
-        <v>0.04292012787180106</v>
+        <v>0.04710129651446118</v>
       </c>
       <c r="CA10">
-        <v>0.9167216040747941</v>
+        <v>1.178400101372425</v>
       </c>
       <c r="CB10">
-        <v>0.4536270913478242</v>
+        <v>0.4611553558822211</v>
       </c>
       <c r="CC10">
-        <v>-0.0001732354369019474</v>
+        <v>0.0005088899298941564</v>
       </c>
       <c r="CD10">
-        <v>0.4593052350187687</v>
+        <v>0.447135198436623</v>
       </c>
       <c r="CE10">
-        <v>-0.06274761746642621</v>
+        <v>-0.04944739260764445</v>
       </c>
       <c r="CF10">
-        <v>0.274416586785724</v>
+        <v>0.698577242014558</v>
       </c>
       <c r="CG10">
-        <v>0.1128579977841335</v>
+        <v>0.09807249550563846</v>
       </c>
       <c r="CH10">
-        <v>0.0006688480118438298</v>
+        <v>-0.0006240649344617842</v>
       </c>
       <c r="CI10">
-        <v>0.09284358662188182</v>
+        <v>0.1156313776464508</v>
       </c>
       <c r="CJ10">
-        <v>0.8576197432008956</v>
+        <v>0.6397601563604972</v>
       </c>
       <c r="CK10">
-        <v>-0.2654004648650376</v>
+        <v>-0.1605026579999047</v>
       </c>
       <c r="CL10">
-        <v>9.303749167643746</v>
+        <v>9.442410896626862</v>
       </c>
       <c r="CM10">
-        <v>-0.03778827452070028</v>
+        <v>-0.02635885447106967</v>
       </c>
       <c r="CN10">
-        <v>10.41475409836066</v>
+        <v>10.20508474576271</v>
       </c>
     </row>
     <row r="11" spans="1:92">
@@ -11782,196 +11836,214 @@
         <v>344</v>
       </c>
       <c r="C47">
-        <v>0.08265964812969791</v>
+        <v>0.04933434531231579</v>
       </c>
       <c r="D47">
-        <v>0.04292076425829271</v>
+        <v>-0.4566932577931364</v>
       </c>
       <c r="E47">
-        <v>0.3502439002193715</v>
+        <v>0.3757131489031663</v>
       </c>
       <c r="F47">
-        <v>0.1025748439718367</v>
+        <v>0.08548033307453555</v>
       </c>
       <c r="G47">
-        <v>0.4643145053914309</v>
+        <v>0.1967785183102628</v>
       </c>
       <c r="H47">
-        <v>0.3463657877006157</v>
+        <v>0.3716280170141263</v>
       </c>
       <c r="I47">
-        <v>-0.1811859868346494</v>
+        <v>-0.1282082648105856</v>
       </c>
       <c r="J47">
-        <v>0.2766076468622292</v>
+        <v>-0.03934652836813769</v>
       </c>
       <c r="K47">
-        <v>0.303390311830642</v>
+        <v>0.2526588339328921</v>
+      </c>
+      <c r="L47">
+        <v>0.06395054454863799</v>
+      </c>
+      <c r="M47">
+        <v>0.6646357150833417</v>
+      </c>
+      <c r="N47">
+        <v>0.4837423983560422</v>
+      </c>
+      <c r="O47">
+        <v>-0.06395054258265551</v>
+      </c>
+      <c r="P47">
+        <v>0.6646356251562832</v>
+      </c>
+      <c r="Q47">
+        <v>0.5162576014286395</v>
       </c>
       <c r="R47">
-        <v>-653.0132560059704</v>
+        <v>-141.7996975441891</v>
       </c>
       <c r="S47">
-        <v>0.6988930805692252</v>
+        <v>0.3341659597316323</v>
       </c>
       <c r="T47">
-        <v>664.8262512438044</v>
+        <v>332.8563184753812</v>
       </c>
       <c r="U47">
-        <v>26.76540965182091</v>
+        <v>6.864197113260457</v>
       </c>
       <c r="V47">
-        <v>-131.7554823086123</v>
+        <v>143.2604034068777</v>
       </c>
       <c r="Z47">
-        <v>0.7355502587619634</v>
+        <v>0.8164895236040338</v>
       </c>
       <c r="AA47">
-        <v>27.31744253524965</v>
+        <v>28.2762393943345</v>
       </c>
       <c r="AE47">
-        <v>0.6901006605697524</v>
+        <v>0.7660386939919104</v>
       </c>
       <c r="AF47">
-        <v>22.21586280532865</v>
+        <v>22.99560268954818</v>
       </c>
       <c r="AK47">
-        <v>25.49714036253216</v>
+        <v>26.39204763885191</v>
       </c>
       <c r="AO47">
-        <v>0.003872516072763511</v>
+        <v>0.004298644131702872</v>
       </c>
       <c r="AP47">
-        <v>0.1432733000100506</v>
+        <v>0.1483019548653907</v>
       </c>
       <c r="AT47">
-        <v>0.003633233579958436</v>
+        <v>0.004033031216433099</v>
       </c>
       <c r="AU47">
-        <v>0.1165167629650104</v>
+        <v>0.1206063078123157</v>
       </c>
       <c r="AZ47">
-        <v>0.1337262606426512</v>
+        <v>0.1384198302736988</v>
       </c>
       <c r="BA47">
-        <v>3.908624452239787</v>
+        <v>2.849787013906935</v>
       </c>
       <c r="BB47">
-        <v>0.23881795298509</v>
+        <v>-0.07869550531905882</v>
       </c>
       <c r="BC47">
-        <v>16.8179233013643</v>
+        <v>17.95042919101711</v>
       </c>
       <c r="BD47">
-        <v>-0.2416226729647127</v>
+        <v>-0.1960013670539986</v>
       </c>
       <c r="BE47">
-        <v>23.96120218579236</v>
+        <v>23.33646616541353</v>
       </c>
       <c r="BF47">
-        <v>2.415004597311695</v>
+        <v>2.107738800822981</v>
       </c>
       <c r="BG47">
-        <v>0.3320138275787093</v>
+        <v>0.09954330516220268</v>
       </c>
       <c r="BH47">
-        <v>6.520213922134452</v>
+        <v>6.996259553238923</v>
       </c>
       <c r="BI47">
-        <v>-0.14281744929147</v>
+        <v>-0.1313738892686262</v>
       </c>
       <c r="BJ47">
-        <v>10.7464480874317</v>
+        <v>10.61278195488722</v>
       </c>
       <c r="BK47">
-        <v>2.346600797261629</v>
+        <v>1.86810247399619</v>
       </c>
       <c r="BL47">
-        <v>0.07925156576485021</v>
+        <v>-0.2478590721108347</v>
       </c>
       <c r="BM47">
-        <v>6.71357038045103</v>
+        <v>7.204612495589292</v>
       </c>
       <c r="BN47">
-        <v>-0.1237288135593221</v>
+        <v>-0.1052973342447028</v>
       </c>
       <c r="BO47">
-        <v>10.36666666666667</v>
+        <v>10.0921052631579</v>
       </c>
       <c r="BP47">
-        <v>-0.8213861294104953</v>
+        <v>-1.059150562442817</v>
       </c>
       <c r="BQ47">
-        <v>0.09737544176765951</v>
+        <v>0.008282737067073408</v>
       </c>
       <c r="BR47">
-        <v>3.567997605615375</v>
+        <v>3.732299514537933</v>
       </c>
       <c r="BS47">
-        <v>0.02333981661572659</v>
+        <v>0.03885850991114145</v>
       </c>
       <c r="BT47">
-        <v>2.878142076502733</v>
+        <v>2.663533834586467</v>
       </c>
       <c r="BU47">
-        <v>0.09293048841948053</v>
+        <v>0.07101354288319581</v>
       </c>
       <c r="BV47">
-        <v>0.512485528713057</v>
+        <v>0.2670116941100222</v>
       </c>
       <c r="BW47">
-        <v>0.3488745267707472</v>
+        <v>0.3742732619501933</v>
       </c>
       <c r="BX47">
-        <v>-0.004405551855266647</v>
+        <v>-0.00317995724487903</v>
       </c>
       <c r="BY47">
-        <v>0.4795977731843611</v>
+        <v>0.4620566743634537</v>
       </c>
       <c r="BZ47">
-        <v>0.08410328280814452</v>
+        <v>0.05304889653688862</v>
       </c>
       <c r="CA47">
-        <v>0.03891443936888834</v>
+        <v>-0.5170399564558569</v>
       </c>
       <c r="CB47">
-        <v>0.363681395712051</v>
+        <v>0.3901853270248822</v>
       </c>
       <c r="CC47">
-        <v>-0.003763438829548545</v>
+        <v>-0.00217839596067916</v>
       </c>
       <c r="CD47">
-        <v>0.4747573747504055</v>
+        <v>0.4496229560030233</v>
       </c>
       <c r="CE47">
-        <v>-0.1724127169049924</v>
+        <v>-0.1136298432228148</v>
       </c>
       <c r="CF47">
-        <v>0.3111184987938847</v>
+        <v>-0.02895197187989974</v>
       </c>
       <c r="CG47">
-        <v>0.285426404074822</v>
+        <v>0.233384201608121</v>
       </c>
       <c r="CH47">
-        <v>0.007971019026021079</v>
+        <v>0.0051319348870346</v>
       </c>
       <c r="CI47">
-        <v>0.04940168266632664</v>
+        <v>0.0923147305357789</v>
       </c>
       <c r="CJ47">
-        <v>2.399323623449664</v>
+        <v>2.114242865113391</v>
       </c>
       <c r="CK47">
-        <v>0.2243123498066195</v>
+        <v>0.0891408181828677</v>
       </c>
       <c r="CL47">
-        <v>7.457771734445814</v>
+        <v>7.925210431350729</v>
       </c>
       <c r="CM47">
-        <v>-0.1758266185051405</v>
+        <v>-0.173274094326726</v>
       </c>
       <c r="CN47">
-        <v>12.65355191256831</v>
+        <v>12.69360902255639</v>
       </c>
     </row>
     <row r="48" spans="1:92">
@@ -16234,202 +16306,220 @@
         <v>9011</v>
       </c>
       <c r="C65">
-        <v>-0.1415700530101933</v>
+        <v>-0.1420493707021763</v>
       </c>
       <c r="D65">
-        <v>-0.4915220012041101</v>
+        <v>-0.2064221155762598</v>
       </c>
       <c r="E65">
-        <v>0.3505341952185676</v>
+        <v>0.3893617274955246</v>
       </c>
       <c r="F65">
-        <v>0.04949202914303881</v>
+        <v>0.05141594900854674</v>
       </c>
       <c r="G65">
-        <v>0.9913825035750545</v>
+        <v>1.314149824877073</v>
       </c>
       <c r="H65">
-        <v>0.3178199231062989</v>
+        <v>0.3529792149415158</v>
       </c>
       <c r="I65">
-        <v>0.1458131826755847</v>
+        <v>0.1486213121882455</v>
       </c>
       <c r="J65">
-        <v>-0.8364305881785409</v>
+        <v>-0.5592112015157437</v>
       </c>
       <c r="K65">
-        <v>0.3316458818844306</v>
+        <v>0.257659057139169</v>
+      </c>
+      <c r="L65">
+        <v>0.0786659134918908</v>
+      </c>
+      <c r="M65">
+        <v>0.2847943647262451</v>
+      </c>
+      <c r="N65">
+        <v>0.4666495748279185</v>
+      </c>
+      <c r="O65">
+        <v>-0.07866590824398238</v>
+      </c>
+      <c r="P65">
+        <v>0.2847944916411569</v>
+      </c>
+      <c r="Q65">
+        <v>0.5333504251750465</v>
       </c>
       <c r="R65">
-        <v>138.2247733069374</v>
+        <v>85.33211705189514</v>
       </c>
       <c r="S65">
-        <v>-0.6492881507536604</v>
+        <v>0.2180548716611285</v>
       </c>
       <c r="T65">
-        <v>433.1177195869698</v>
+        <v>356.7282412170728</v>
       </c>
       <c r="U65">
-        <v>-5.137490295118418</v>
+        <v>-0.849583643994927</v>
       </c>
       <c r="V65">
-        <v>583.2807931544373</v>
+        <v>379.5840592510853</v>
       </c>
       <c r="Z65">
-        <v>0.891919161043667</v>
+        <v>1.046101686127638</v>
       </c>
       <c r="AA65">
-        <v>29.09040824484682</v>
+        <v>30.66398270595238</v>
       </c>
       <c r="AE65">
-        <v>0.900904846728169</v>
+        <v>1.056640691629629</v>
       </c>
       <c r="AF65">
-        <v>34.81381696757556</v>
+        <v>36.69698522058502</v>
       </c>
       <c r="AJ65">
-        <v>1.328443771596773</v>
+        <v>1.558086573414366</v>
       </c>
       <c r="AK65">
-        <v>29.04737509655563</v>
+        <v>30.61862178478972</v>
       </c>
       <c r="AO65">
-        <v>0.003671204614297868</v>
+        <v>0.00430583118389643</v>
       </c>
       <c r="AP65">
-        <v>0.1186153241380095</v>
+        <v>0.1250315298917528</v>
       </c>
       <c r="AT65">
-        <v>0.003708190354921461</v>
+        <v>0.0043492105026945</v>
       </c>
       <c r="AU65">
-        <v>0.1419523627627954</v>
+        <v>0.1496309285243018</v>
       </c>
       <c r="AY65">
-        <v>0.005467971893792029</v>
+        <v>0.006413198491106671</v>
       </c>
       <c r="AZ65">
-        <v>0.118439857682184</v>
+        <v>0.1248465720072976</v>
       </c>
       <c r="BA65">
-        <v>-2.305242374589922</v>
+        <v>-1.740760819216694</v>
       </c>
       <c r="BB65">
-        <v>-0.9371975927514349</v>
+        <v>-0.3063060096543673</v>
       </c>
       <c r="BC65">
-        <v>13.08570333861962</v>
+        <v>14.0087980266542</v>
       </c>
       <c r="BD65">
-        <v>0.03209224784662395</v>
+        <v>-0.02519534972365178</v>
       </c>
       <c r="BE65">
-        <v>12.16994535519127</v>
+        <v>14.68619528619529</v>
       </c>
       <c r="BF65">
-        <v>-0.661667005114749</v>
+        <v>-0.4712008016794442</v>
       </c>
       <c r="BG65">
-        <v>-1.383086066280345</v>
+        <v>-0.9948644078573503</v>
       </c>
       <c r="BH65">
-        <v>4.822499262815919</v>
+        <v>5.363052053236021</v>
       </c>
       <c r="BI65">
-        <v>0.03050847457627112</v>
+        <v>-0.0006098723079855535</v>
       </c>
       <c r="BJ65">
-        <v>3.933333333333337</v>
+        <v>5.386531986531986</v>
       </c>
       <c r="BK65">
-        <v>-2.381921443927601</v>
+        <v>-2.240183863204612</v>
       </c>
       <c r="BL65">
-        <v>-0.8092588030405182</v>
+        <v>-0.3708365574906378</v>
       </c>
       <c r="BM65">
-        <v>5.421267043487493</v>
+        <v>6.02200311185707</v>
       </c>
       <c r="BN65">
-        <v>0.06499027507641005</v>
+        <v>0.04002287021154942</v>
       </c>
       <c r="BO65">
-        <v>3.532786885245905</v>
+        <v>4.976430976430976</v>
       </c>
       <c r="BP65">
-        <v>0.6544491455988427</v>
+        <v>0.9665526955008881</v>
       </c>
       <c r="BQ65">
-        <v>-0.9088351907593279</v>
+        <v>-0.7834373325143476</v>
       </c>
       <c r="BR65">
-        <v>2.841937031882113</v>
+        <v>2.623742860256491</v>
       </c>
       <c r="BS65">
-        <v>-0.06340650180605724</v>
+        <v>-0.0646083476272156</v>
       </c>
       <c r="BT65">
-        <v>4.703825136612022</v>
+        <v>4.323232323232324</v>
       </c>
       <c r="BU65">
-        <v>0.04398692915666234</v>
+        <v>0.04845561027024558</v>
       </c>
       <c r="BV65">
-        <v>0.3839366256979521</v>
+        <v>0.4492345122308752</v>
       </c>
       <c r="BW65">
-        <v>0.3288662038112434</v>
+        <v>0.3653223231161853</v>
       </c>
       <c r="BX65">
-        <v>0.002494807001383256</v>
+        <v>0.0005368789695481436</v>
       </c>
       <c r="BY65">
-        <v>0.2555440028418764</v>
+        <v>0.3514847177321767</v>
       </c>
       <c r="BZ65">
-        <v>-0.1520020046179072</v>
+        <v>-0.1378078235456782</v>
       </c>
       <c r="CA65">
-        <v>-0.7340122425270671</v>
+        <v>-0.3678050298685199</v>
       </c>
       <c r="CB65">
-        <v>0.382330051144149</v>
+        <v>0.4231335885403462</v>
       </c>
       <c r="CC65">
-        <v>0.006259691348017826</v>
+        <v>0.005152687661622438</v>
       </c>
       <c r="CD65">
-        <v>0.1993661422945671</v>
+        <v>0.2875049821671612</v>
       </c>
       <c r="CE65">
-        <v>0.1385234615014661</v>
+        <v>0.1104487407163886</v>
       </c>
       <c r="CF65">
-        <v>-1.023576605117593</v>
+        <v>-0.6934054006232365</v>
       </c>
       <c r="CG65">
-        <v>0.2888037448014081</v>
+        <v>0.2115440882247533</v>
       </c>
       <c r="CH65">
-        <v>-0.008754498349401093</v>
+        <v>-0.005689566631170593</v>
       </c>
       <c r="CI65">
-        <v>0.545089854863557</v>
+        <v>0.3610103001006619</v>
       </c>
       <c r="CJ65">
-        <v>-1.828395367987583</v>
+        <v>-1.679980682377926</v>
       </c>
       <c r="CK65">
-        <v>-0.4963669911515479</v>
+        <v>0.1216352577311278</v>
       </c>
       <c r="CL65">
-        <v>6.102154262446162</v>
+        <v>6.670441506703358</v>
       </c>
       <c r="CM65">
-        <v>0.03603778827452066</v>
+        <v>0.004116638078902172</v>
       </c>
       <c r="CN65">
-        <v>5.053551912568309</v>
+        <v>6.557575757575757</v>
       </c>
     </row>
     <row r="66" spans="1:92">

</xml_diff>